<commit_message>
Actualizacion para empezar doc Tesis 2
</commit_message>
<xml_diff>
--- a/Codigo/Version V2.1/Datos/Data.xlsx
+++ b/Codigo/Version V2.1/Datos/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rozog\OneDrive\Escritorio\Cinetica Propia\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rozog\OneDrive - Universidad de los Andes\Duodecimo semestre\Repositorio_Maestria\Codigo\Version V2.1\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{38668F12-C913-44DA-A828-623EC47DB50C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{0091112E-1ED1-462C-A14B-48C71FCBF0F2}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{E94D89DB-EDD3-4648-A7FA-32DBE5122644}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D14C8C16-144E-490F-A701-817670609726}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{376766A5-389D-4DCC-947A-B711BF4B8F7C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{376766A5-389D-4DCC-947A-B711BF4B8F7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -430,15 +430,15 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -455,25 +455,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <v>8.6999999999999993</v>
+        <v>1.5</v>
       </c>
       <c r="C2" s="1">
         <v>36400</v>
       </c>
       <c r="D2" s="2">
-        <v>2.5000000000000002E-6</v>
+        <v>1.4800000000000001E-9</v>
       </c>
       <c r="E2" s="1">
-        <f>36400</f>
-        <v>36400</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+        <f>6700</f>
+        <v>6700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -490,7 +490,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -508,7 +508,7 @@
         <v>-1700</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -526,7 +526,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -544,7 +544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -562,7 +562,7 @@
         <v>-31400</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>